<commit_message>
update for deploy on star computer
</commit_message>
<xml_diff>
--- a/LSI Evaluation.xlsx
+++ b/LSI Evaluation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hester/Desktop/finalYearProject/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quanyewu/Desktop/Final-Year-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,90 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>os</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fibonacci</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cluster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>naïve_bayes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KNN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regresion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CNN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>euclidean distance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>entropy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MPI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LSA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tensorflow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vggish_slim.define_vggish_slim()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random.randint()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data_provider.provide_data()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hashlib.md5()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Precision@10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>numpy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -54,7 +138,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>os</t>
+    <t>graph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PANDAS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -66,30 +158,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>parsing tree</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>graph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>map reduce</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PANDAS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>remove</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pop</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -114,87 +190,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>recursion</t>
+    <t>socket</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>binary search</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fibonacci</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cluster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>naïve_bayes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KNN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>regresion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CNN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>euclidean distance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>entropy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>database</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MPI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SVD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LSA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tensorflow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vggish_slim.define_vggish_slim()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>random.randint()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data_provider.provide_data()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hashlib.md5()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Precision@10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27" x14ac:dyDescent="0.3"/>
@@ -563,208 +563,334 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2">
         <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="B9" s="2">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update for final-version:local version
</commit_message>
<xml_diff>
--- a/LSI Evaluation.xlsx
+++ b/LSI Evaluation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>query</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,6 +38,122 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>SVD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LSA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tensorflow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vggish_slim.define_vggish_slim()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random.randint()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data_provider.provide_data()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hashlib.md5()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Precision@10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>numpy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scipy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sklearn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ast</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>graph</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clock</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parsing tree</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>append</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>socket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>binary search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insertion sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heap sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>matplotlib.pyplot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>merge sort</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PANDAS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>fibonacci</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -46,7 +162,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>naïve_bayes</t>
+    <t>notes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tensorflow also returned</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -54,7 +174,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>regresion</t>
+    <t>regression</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -70,7 +190,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>database</t>
+    <t>database connection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -78,123 +198,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>naïve bayes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>PCA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SVD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LSA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tensorflow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vggish_slim.define_vggish_slim()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>random.randint()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data_provider.provide_data()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hashlib.md5()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Precision@10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>numpy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>scipy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sklearn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ast</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>graph</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PANDAS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>remove</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>clock</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>merge sort</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>parsing tree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>append</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>matplotlib.pyplot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>redis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insertion sort</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>heap sort</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>socket</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>binary search</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -543,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27" x14ac:dyDescent="0.3"/>
@@ -552,7 +560,8 @@
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
     <col min="2" max="2" width="63.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="45.33203125" style="2" customWidth="1"/>
-    <col min="4" max="7" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="44.83203125" style="2" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -563,13 +572,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>10</v>
@@ -580,7 +592,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>6</v>
@@ -591,7 +603,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
@@ -602,7 +614,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>10</v>
@@ -613,7 +625,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>10</v>
@@ -635,7 +647,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>10</v>
@@ -646,7 +658,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>10</v>
@@ -657,18 +669,18 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2">
-        <v>0.3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -679,7 +691,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <v>7</v>
@@ -690,18 +702,18 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13" s="2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <v>8</v>
@@ -712,7 +724,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B15" s="2">
         <v>3</v>
@@ -723,7 +735,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>8</v>
@@ -732,165 +744,228 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="2">
-        <v>10</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="B27" s="2">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="B28" s="2">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="2">
-        <v>10</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="B29" s="2">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="B31" s="2">
+        <v>10</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="2">
-        <v>10</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="B32" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>11</v>
+      <c r="C32" s="2">
+        <v>0.9</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>